<commit_message>
enhanced state vehicle variable, still needs review for mag and baro
</commit_message>
<xml_diff>
--- a/AeroQuad_ICD.xlsx
+++ b/AeroQuad_ICD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495" activeTab="1"/>
+    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Serial" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
   <si>
     <t>Commands</t>
   </si>
@@ -359,18 +359,9 @@
     <t>CAMERASTABLE_ENABLED</t>
   </si>
   <si>
-    <t>Flight Configuration</t>
-  </si>
-  <si>
     <t>Board Type</t>
   </si>
   <si>
-    <t>Receiver Channel Count</t>
-  </si>
-  <si>
-    <t>Motor Count</t>
-  </si>
-  <si>
     <t>ALTITUDEHOLD_ENABLED</t>
   </si>
   <si>
@@ -603,6 +594,9 @@
   </si>
   <si>
     <t>11111</t>
+  </si>
+  <si>
+    <t>read vehicle state variable</t>
   </si>
 </sst>
 </file>
@@ -626,18 +620,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -652,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -675,61 +663,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,60 +683,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -806,6 +732,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:C33" totalsRowShown="0">
+  <autoFilter ref="B2:C33"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Value" dataDxfId="2"/>
+    <tableColumn id="2" name="Commands" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="E2:F33" totalsRowShown="0">
+  <autoFilter ref="E2:F33"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Value" dataDxfId="0"/>
+    <tableColumn id="2" name="Telemetry"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1055,7 @@
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -1397,7 +1345,9 @@
       <c r="E19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -1561,17 +1511,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1579,53 +1536,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="6" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
-      <c r="F1" s="15"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="F2" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1640,14 +1598,14 @@
       <c r="D4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>122</v>
+      <c r="F4" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>127</v>
+      <c r="H4" s="14" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1661,12 +1619,12 @@
       <c r="D5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>123</v>
+      <c r="F5" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1680,12 +1638,12 @@
       <c r="D6" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>125</v>
+      <c r="F6" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1699,193 +1657,237 @@
       <c r="D7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>124</v>
+      <c r="F7" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>126</v>
+      <c r="C8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="18" t="s">
-        <v>131</v>
+      <c r="H8" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="17" t="s">
-        <v>137</v>
+      <c r="C9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="22"/>
-      <c r="F10" s="17" t="s">
-        <v>138</v>
+      <c r="C10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="22"/>
-      <c r="F11" s="17" t="s">
-        <v>139</v>
+      <c r="C11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="18" t="s">
-        <v>134</v>
+      <c r="H11" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>140</v>
+      <c r="C12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="26"/>
-      <c r="F13" s="17" t="s">
-        <v>141</v>
+      <c r="C13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="F13" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="F14" s="17" t="s">
-        <v>142</v>
+      <c r="C14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="F14" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>11</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="26"/>
-      <c r="F15" s="17" t="s">
-        <v>143</v>
+      <c r="C15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="F15" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="27"/>
-      <c r="F16" s="17" t="s">
-        <v>144</v>
+      <c r="C16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="F16" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>13</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>145</v>
+      <c r="C17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="F17" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>14</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9"/>
-      <c r="F18" s="17" t="s">
-        <v>146</v>
+      <c r="C18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="10"/>
-      <c r="F19" s="17" t="s">
-        <v>147</v>
+      <c r="C19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="F19" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>16</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1895,14 +1897,12 @@
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
@@ -1912,14 +1912,14 @@
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="F22" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="G22" s="13" t="s">
+      <c r="D22" s="7"/>
+      <c r="F22" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1931,13 +1931,13 @@
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="F23" s="17" t="s">
-        <v>164</v>
+      <c r="D23" s="7"/>
+      <c r="F23" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="18" t="s">
-        <v>150</v>
+      <c r="H23" s="14" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1948,15 +1948,13 @@
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>165</v>
+      <c r="D24" s="7"/>
+      <c r="F24" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1967,15 +1965,13 @@
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>166</v>
+      <c r="D25" s="7"/>
+      <c r="F25" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1986,15 +1982,13 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>167</v>
+      <c r="D26" s="7"/>
+      <c r="F26" s="13" t="s">
+        <v>164</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -2005,15 +1999,13 @@
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>168</v>
+      <c r="D27" s="7"/>
+      <c r="F27" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="18" t="s">
-        <v>154</v>
+      <c r="H27" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -2024,15 +2016,13 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>169</v>
+      <c r="D28" s="7"/>
+      <c r="F28" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -2044,12 +2034,12 @@
         <v>2000000</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="F29" s="17" t="s">
-        <v>170</v>
+      <c r="F29" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -2061,12 +2051,12 @@
         <v>4000000</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="F30" s="17" t="s">
-        <v>171</v>
+      <c r="F30" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="18" t="s">
-        <v>158</v>
+      <c r="H30" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -2078,12 +2068,12 @@
         <v>8000000</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="F31" s="17" t="s">
-        <v>172</v>
+      <c r="F31" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="23" t="s">
-        <v>157</v>
+      <c r="H31" s="15" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -2095,12 +2085,12 @@
         <v>10000000</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="F32" s="17" t="s">
-        <v>173</v>
+      <c r="F32" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="23" t="s">
-        <v>159</v>
+      <c r="H32" s="15" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -2112,12 +2102,12 @@
         <v>20000000</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="F33" s="17" t="s">
-        <v>174</v>
+      <c r="F33" s="13" t="s">
+        <v>171</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="23" t="s">
-        <v>160</v>
+      <c r="H33" s="15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -2129,12 +2119,12 @@
         <v>40000000</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="F34" s="17" t="s">
-        <v>175</v>
+      <c r="F34" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="23" t="s">
-        <v>161</v>
+      <c r="H34" s="15" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -2146,192 +2136,190 @@
         <v>80000000</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="F35" s="17" t="s">
-        <v>176</v>
+      <c r="F35" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="23" t="s">
-        <v>162</v>
+      <c r="H35" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="17" t="s">
-        <v>177</v>
+      <c r="F36" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="17" t="s">
-        <v>178</v>
+      <c r="F37" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F38" s="17" t="s">
-        <v>179</v>
+      <c r="F38" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F39" s="17" t="s">
-        <v>180</v>
+      <c r="F39" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F40" s="17" t="s">
-        <v>181</v>
+      <c r="F40" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F41" s="17" t="s">
-        <v>182</v>
+      <c r="F41" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F42" s="17" t="s">
-        <v>183</v>
+      <c r="F42" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F43" s="17" t="s">
-        <v>184</v>
+      <c r="F43" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="17" t="s">
-        <v>185</v>
+      <c r="F44" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="17" t="s">
-        <v>186</v>
+      <c r="F45" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="17" t="s">
-        <v>187</v>
+      <c r="F46" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F47" s="17" t="s">
-        <v>188</v>
+      <c r="F47" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="17" t="s">
-        <v>189</v>
+      <c r="F48" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F49" s="17" t="s">
-        <v>190</v>
+      <c r="F49" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F50" s="17" t="s">
-        <v>191</v>
+      <c r="F50" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="17" t="s">
-        <v>192</v>
+      <c r="F51" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="17" t="s">
-        <v>193</v>
+      <c r="F52" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F53" s="17" t="s">
-        <v>194</v>
+      <c r="F53" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F54" s="17" t="s">
-        <v>195</v>
+      <c r="F54" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Sync experimental from v3.0
</commit_message>
<xml_diff>
--- a/AeroQuad_ICD.xlsx
+++ b/AeroQuad_ICD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495" activeTab="1"/>
+    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Serial" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
   <si>
     <t>Commands</t>
   </si>
@@ -359,18 +359,9 @@
     <t>CAMERASTABLE_ENABLED</t>
   </si>
   <si>
-    <t>Flight Configuration</t>
-  </si>
-  <si>
     <t>Board Type</t>
   </si>
   <si>
-    <t>Receiver Channel Count</t>
-  </si>
-  <si>
-    <t>Motor Count</t>
-  </si>
-  <si>
     <t>ALTITUDEHOLD_ENABLED</t>
   </si>
   <si>
@@ -603,6 +594,9 @@
   </si>
   <si>
     <t>11111</t>
+  </si>
+  <si>
+    <t>read vehicle state variable</t>
   </si>
 </sst>
 </file>
@@ -626,18 +620,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -652,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -675,61 +663,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,60 +683,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -806,6 +732,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:C33" totalsRowShown="0">
+  <autoFilter ref="B2:C33"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Value" dataDxfId="2"/>
+    <tableColumn id="2" name="Commands" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="E2:F33" totalsRowShown="0">
+  <autoFilter ref="E2:F33"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Value" dataDxfId="0"/>
+    <tableColumn id="2" name="Telemetry"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1055,7 @@
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -1397,7 +1345,9 @@
       <c r="E19" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -1561,17 +1511,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1579,53 +1536,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="6" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
-      <c r="F1" s="15"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="F2" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1640,14 +1598,14 @@
       <c r="D4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>122</v>
+      <c r="F4" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>127</v>
+      <c r="H4" s="14" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1661,12 +1619,12 @@
       <c r="D5" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>123</v>
+      <c r="F5" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1680,12 +1638,12 @@
       <c r="D6" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>125</v>
+      <c r="F6" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1699,193 +1657,237 @@
       <c r="D7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>124</v>
+      <c r="F7" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>126</v>
+      <c r="C8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="18" t="s">
-        <v>131</v>
+      <c r="H8" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="17" t="s">
-        <v>137</v>
+      <c r="C9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="22"/>
-      <c r="F10" s="17" t="s">
-        <v>138</v>
+      <c r="C10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="22"/>
-      <c r="F11" s="17" t="s">
-        <v>139</v>
+      <c r="C11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="18" t="s">
-        <v>134</v>
+      <c r="H11" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>140</v>
+      <c r="C12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="26"/>
-      <c r="F13" s="17" t="s">
-        <v>141</v>
+      <c r="C13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="F13" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="F14" s="17" t="s">
-        <v>142</v>
+      <c r="C14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="F14" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>11</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="26"/>
-      <c r="F15" s="17" t="s">
-        <v>143</v>
+      <c r="C15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="F15" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="27"/>
-      <c r="F16" s="17" t="s">
-        <v>144</v>
+      <c r="C16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="F16" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>13</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>145</v>
+      <c r="C17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="F17" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>14</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9"/>
-      <c r="F18" s="17" t="s">
-        <v>146</v>
+      <c r="C18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="10"/>
-      <c r="F19" s="17" t="s">
-        <v>147</v>
+      <c r="C19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="F19" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>16</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1895,14 +1897,12 @@
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
@@ -1912,14 +1912,14 @@
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="F22" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="G22" s="13" t="s">
+      <c r="D22" s="7"/>
+      <c r="F22" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1931,13 +1931,13 @@
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="F23" s="17" t="s">
-        <v>164</v>
+      <c r="D23" s="7"/>
+      <c r="F23" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="18" t="s">
-        <v>150</v>
+      <c r="H23" s="14" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1948,15 +1948,13 @@
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>165</v>
+      <c r="D24" s="7"/>
+      <c r="F24" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1967,15 +1965,13 @@
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>166</v>
+      <c r="D25" s="7"/>
+      <c r="F25" s="13" t="s">
+        <v>163</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1986,15 +1982,13 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>167</v>
+      <c r="D26" s="7"/>
+      <c r="F26" s="13" t="s">
+        <v>164</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -2005,15 +1999,13 @@
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>168</v>
+      <c r="D27" s="7"/>
+      <c r="F27" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="18" t="s">
-        <v>154</v>
+      <c r="H27" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -2024,15 +2016,13 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>169</v>
+      <c r="D28" s="7"/>
+      <c r="F28" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -2044,12 +2034,12 @@
         <v>2000000</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="F29" s="17" t="s">
-        <v>170</v>
+      <c r="F29" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -2061,12 +2051,12 @@
         <v>4000000</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="F30" s="17" t="s">
-        <v>171</v>
+      <c r="F30" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="18" t="s">
-        <v>158</v>
+      <c r="H30" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -2078,12 +2068,12 @@
         <v>8000000</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="F31" s="17" t="s">
-        <v>172</v>
+      <c r="F31" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="23" t="s">
-        <v>157</v>
+      <c r="H31" s="15" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -2095,12 +2085,12 @@
         <v>10000000</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="F32" s="17" t="s">
-        <v>173</v>
+      <c r="F32" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="23" t="s">
-        <v>159</v>
+      <c r="H32" s="15" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -2112,12 +2102,12 @@
         <v>20000000</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="F33" s="17" t="s">
-        <v>174</v>
+      <c r="F33" s="13" t="s">
+        <v>171</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="23" t="s">
-        <v>160</v>
+      <c r="H33" s="15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -2129,12 +2119,12 @@
         <v>40000000</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="F34" s="17" t="s">
-        <v>175</v>
+      <c r="F34" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="23" t="s">
-        <v>161</v>
+      <c r="H34" s="15" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -2146,192 +2136,190 @@
         <v>80000000</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="F35" s="17" t="s">
-        <v>176</v>
+      <c r="F35" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="23" t="s">
-        <v>162</v>
+      <c r="H35" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="17" t="s">
-        <v>177</v>
+      <c r="F36" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="17" t="s">
-        <v>178</v>
+      <c r="F37" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F38" s="17" t="s">
-        <v>179</v>
+      <c r="F38" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F39" s="17" t="s">
-        <v>180</v>
+      <c r="F39" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F40" s="17" t="s">
-        <v>181</v>
+      <c r="F40" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F41" s="17" t="s">
-        <v>182</v>
+      <c r="F41" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F42" s="17" t="s">
-        <v>183</v>
+      <c r="F42" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F43" s="17" t="s">
-        <v>184</v>
+      <c r="F43" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="17" t="s">
-        <v>185</v>
+      <c r="F44" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="17" t="s">
-        <v>186</v>
+      <c r="F45" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="17" t="s">
-        <v>187</v>
+      <c r="F46" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F47" s="17" t="s">
-        <v>188</v>
+      <c r="F47" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="17" t="s">
-        <v>189</v>
+      <c r="F48" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F49" s="17" t="s">
-        <v>190</v>
+      <c r="F49" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F50" s="17" t="s">
-        <v>191</v>
+      <c r="F50" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="17" t="s">
-        <v>192</v>
+      <c r="F51" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="17" t="s">
-        <v>193</v>
+      <c r="F52" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F53" s="17" t="s">
-        <v>194</v>
+      <c r="F53" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F54" s="17" t="s">
-        <v>195</v>
+      <c r="F54" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added min/max range finder values
</commit_message>
<xml_diff>
--- a/AeroQuad_ICD.xlsx
+++ b/AeroQuad_ICD.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="196">
   <si>
     <t>Commands</t>
   </si>
@@ -597,6 +597,12 @@
   </si>
   <si>
     <t>read vehicle state variable</t>
+  </si>
+  <si>
+    <t>range finder</t>
+  </si>
+  <si>
+    <t>read range finder</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,12 +1400,16 @@
       <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>

</xml_diff>